<commit_message>
added new constraint algorithm (lots of changes)
</commit_message>
<xml_diff>
--- a/afccp/resources/shared/real/Value_Parameters_Defaults_2023.xlsx
+++ b/afccp/resources/shared/real/Value_Parameters_Defaults_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griffenlaird/Desktop/Coding Projects/afccp/afccp/resources/shared/real/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B53449-4613-9049-9A17-60B94F7FF62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99160771-CEC3-DF40-89BB-7154494C7514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="30260" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="24840" windowHeight="17480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Weights" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>AFSC Weight Function</t>
   </si>
   <si>
-    <t>Linear</t>
-  </si>
-  <si>
     <t>Piece</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>0.8, 5</t>
+  </si>
+  <si>
+    <t>Curve_1</t>
   </si>
 </sst>
 </file>
@@ -780,9 +780,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -806,10 +813,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="B2">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -818,10 +825,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -833,24 +840,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>55.49</v>
@@ -861,7 +870,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>55.49</v>
@@ -872,7 +881,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>88.82</v>
@@ -883,7 +892,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>55.49</v>
@@ -894,7 +903,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -905,7 +914,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>66.67</v>
@@ -916,7 +925,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>66.67</v>
@@ -927,7 +936,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -938,7 +947,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>77.64</v>
@@ -949,7 +958,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>66.67</v>
@@ -960,7 +969,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>77.64</v>
@@ -971,7 +980,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>66.67</v>
@@ -982,7 +991,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>55.49</v>
@@ -993,7 +1002,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>55.49</v>
@@ -1004,7 +1013,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>55.49</v>
@@ -1015,7 +1024,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>55.49</v>
@@ -1026,7 +1035,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>66.67</v>
@@ -1037,7 +1046,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>55.49</v>
@@ -1048,7 +1057,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>55.49</v>
@@ -1059,7 +1068,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>77.64</v>
@@ -1070,7 +1079,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>55.49</v>
@@ -1081,7 +1090,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>55.49</v>
@@ -1092,7 +1101,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>55.49</v>
@@ -1103,7 +1112,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>55.49</v>
@@ -1114,7 +1123,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>55.49</v>
@@ -1125,7 +1134,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>77.64</v>
@@ -1136,7 +1145,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>66.67</v>
@@ -1147,7 +1156,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>55.49</v>
@@ -1158,7 +1167,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>55.49</v>
@@ -1169,7 +1178,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>77.64</v>
@@ -1180,7 +1189,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>77.64</v>
@@ -1191,7 +1200,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>66.67</v>
@@ -1209,53 +1218,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1293,7 +1302,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1331,7 +1340,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>30.00000086999999</v>
@@ -1369,7 +1378,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1407,7 +1416,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>30</v>
@@ -1445,7 +1454,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1483,7 +1492,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1521,7 +1530,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>30</v>
@@ -1559,7 +1568,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>29.999999729999999</v>
@@ -1597,7 +1606,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1635,7 +1644,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>29.999999729999999</v>
@@ -1673,7 +1682,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1711,7 +1720,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1749,7 +1758,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1787,7 +1796,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1825,7 +1834,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1863,7 +1872,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>30.000000300000011</v>
@@ -1901,7 +1910,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1939,7 +1948,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1977,7 +1986,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>30</v>
@@ -2015,7 +2024,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2053,7 +2062,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2091,7 +2100,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2129,7 +2138,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2167,7 +2176,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2205,13 +2214,13 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <v>100</v>
@@ -2243,7 +2252,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2281,7 +2290,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -2319,7 +2328,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -2357,7 +2366,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>30.000000300000011</v>
@@ -2395,7 +2404,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>29.999999729999999</v>
@@ -2433,7 +2442,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -2479,52 +2488,52 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0.50095019880045821</v>
@@ -2562,7 +2571,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0.50095019880045821</v>
@@ -2600,7 +2609,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>0.50000171807800331</v>
@@ -2638,7 +2647,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0.50095019880045821</v>
@@ -2676,7 +2685,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0.50000171807800331</v>
@@ -2714,7 +2723,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>0.50095019880045821</v>
@@ -2752,7 +2761,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>0.50095019880045821</v>
@@ -2790,7 +2799,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>0.50000171807800331</v>
@@ -2828,7 +2837,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>0.50000171807800331</v>
@@ -2866,7 +2875,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>0.50095019880045821</v>
@@ -2904,7 +2913,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>0.50000171807800331</v>
@@ -2942,7 +2951,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>0.50095019880045821</v>
@@ -2980,7 +2989,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>0.50095019880045821</v>
@@ -3018,7 +3027,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>0.50095019880045821</v>
@@ -3056,7 +3065,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>0.50095019880045821</v>
@@ -3094,7 +3103,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0.50095019880045821</v>
@@ -3132,7 +3141,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>0.50000171807800331</v>
@@ -3170,7 +3179,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>0.50095019880045821</v>
@@ -3208,7 +3217,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>0.50095019880045821</v>
@@ -3246,7 +3255,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>0.50000171807800331</v>
@@ -3284,7 +3293,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>0.50095019880045821</v>
@@ -3322,7 +3331,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>0.50095019880045821</v>
@@ -3360,7 +3369,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>0.50095019880045821</v>
@@ -3398,7 +3407,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>0.50095019880045821</v>
@@ -3436,7 +3445,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>0.50095019880045821</v>
@@ -3474,7 +3483,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>0.50095019880045821</v>
@@ -3512,7 +3521,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>0.50095019880045821</v>
@@ -3550,7 +3559,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>0.50095019880045821</v>
@@ -3588,7 +3597,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>0.50095019880045821</v>
@@ -3626,7 +3635,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>0.50000171807800331</v>
@@ -3664,7 +3673,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>0.50000171807800331</v>
@@ -3702,7 +3711,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>0.50095019880045821</v>
@@ -3747,53 +3756,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3802,36 +3811,36 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
-      </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3840,74 +3849,74 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
-      </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3916,74 +3925,74 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
         <v>60</v>
       </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>61</v>
-      </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
         <v>117</v>
       </c>
-      <c r="C6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" t="s">
-        <v>118</v>
-      </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3992,36 +4001,36 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4030,112 +4039,112 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
         <v>64</v>
       </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" t="s">
-        <v>65</v>
-      </c>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4144,74 +4153,74 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4220,36 +4229,36 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4258,36 +4267,36 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" t="s">
         <v>71</v>
       </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>72</v>
-      </c>
       <c r="H14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4296,36 +4305,36 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4334,36 +4343,36 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4372,74 +4381,74 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4448,36 +4457,36 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -4486,74 +4495,74 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -4562,36 +4571,36 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4600,36 +4609,36 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -4638,36 +4647,36 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -4676,36 +4685,36 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -4714,36 +4723,36 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4752,36 +4761,36 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -4790,36 +4799,36 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4828,36 +4837,36 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4866,112 +4875,112 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" t="s">
         <v>87</v>
       </c>
-      <c r="E31" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" t="s">
-        <v>88</v>
-      </c>
       <c r="H31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -4980,31 +4989,31 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -5017,52 +5026,55 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5100,7 +5112,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5138,7 +5150,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -5176,7 +5188,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5214,7 +5226,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -5252,7 +5264,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5290,7 +5302,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5328,7 +5340,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -5366,7 +5378,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -5404,7 +5416,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -5442,7 +5454,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -5480,7 +5492,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -5518,7 +5530,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -5556,7 +5568,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -5594,7 +5606,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5632,7 +5644,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5670,7 +5682,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5708,7 +5720,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5746,7 +5758,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -5784,7 +5796,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5822,7 +5834,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -5860,7 +5872,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -5898,7 +5910,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5936,7 +5948,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -5974,7 +5986,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -6012,7 +6024,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -6050,7 +6062,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -6088,7 +6100,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -6126,7 +6138,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -6164,7 +6176,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -6202,7 +6214,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -6240,7 +6252,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -6286,7 +6298,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6299,1256 +6311,1256 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" t="s">
         <v>93</v>
       </c>
-      <c r="F2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>94</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>95</v>
       </c>
-      <c r="J2" t="s">
-        <v>96</v>
-      </c>
       <c r="K2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
         <v>91</v>
       </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>92</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
         <v>93</v>
       </c>
-      <c r="F3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>94</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>95</v>
       </c>
-      <c r="J3" t="s">
-        <v>96</v>
-      </c>
       <c r="K3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
         <v>93</v>
       </c>
-      <c r="F4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>94</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>95</v>
       </c>
-      <c r="J4" t="s">
-        <v>96</v>
-      </c>
       <c r="K4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" t="s">
         <v>95</v>
       </c>
-      <c r="J5" t="s">
-        <v>96</v>
-      </c>
       <c r="K5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" t="s">
         <v>93</v>
       </c>
-      <c r="F6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>94</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>95</v>
       </c>
-      <c r="J6" t="s">
-        <v>96</v>
-      </c>
       <c r="K6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" t="s">
         <v>95</v>
       </c>
-      <c r="J7" t="s">
-        <v>96</v>
-      </c>
       <c r="K7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" t="s">
         <v>93</v>
       </c>
-      <c r="F8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>94</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>95</v>
       </c>
-      <c r="J8" t="s">
-        <v>96</v>
-      </c>
       <c r="K8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J9" t="s">
         <v>95</v>
       </c>
-      <c r="J9" t="s">
-        <v>96</v>
-      </c>
       <c r="K9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H10" t="s">
         <v>93</v>
       </c>
-      <c r="F10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>94</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>95</v>
       </c>
-      <c r="J10" t="s">
-        <v>96</v>
-      </c>
       <c r="K10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
         <v>91</v>
       </c>
-      <c r="C11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>92</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" t="s">
         <v>93</v>
       </c>
-      <c r="F11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>94</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>95</v>
       </c>
-      <c r="J11" t="s">
-        <v>96</v>
-      </c>
       <c r="K11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" t="s">
         <v>93</v>
       </c>
-      <c r="F12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" t="s">
-        <v>115</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>94</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>95</v>
       </c>
-      <c r="J12" t="s">
-        <v>96</v>
-      </c>
       <c r="K12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H13" t="s">
         <v>93</v>
       </c>
-      <c r="F13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" t="s">
-        <v>115</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>94</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>95</v>
       </c>
-      <c r="J13" t="s">
-        <v>96</v>
-      </c>
       <c r="K13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" t="s">
         <v>95</v>
       </c>
-      <c r="D14" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" t="s">
-        <v>115</v>
-      </c>
-      <c r="H14" t="s">
-        <v>94</v>
-      </c>
-      <c r="I14" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14" t="s">
-        <v>96</v>
-      </c>
       <c r="K14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
         <v>91</v>
       </c>
-      <c r="C15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>92</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" t="s">
         <v>93</v>
       </c>
-      <c r="F15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" t="s">
-        <v>115</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>94</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>95</v>
       </c>
-      <c r="J15" t="s">
-        <v>96</v>
-      </c>
       <c r="K15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" t="s">
         <v>91</v>
       </c>
-      <c r="C16" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>92</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" t="s">
         <v>93</v>
       </c>
-      <c r="F16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>94</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>95</v>
       </c>
-      <c r="J16" t="s">
-        <v>96</v>
-      </c>
       <c r="K16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
         <v>91</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" t="s">
         <v>95</v>
       </c>
-      <c r="D17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" t="s">
-        <v>115</v>
-      </c>
-      <c r="H17" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" t="s">
-        <v>96</v>
-      </c>
       <c r="K17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
         <v>91</v>
       </c>
-      <c r="C18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>92</v>
       </c>
-      <c r="E18" t="s">
-        <v>93</v>
-      </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I18" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" t="s">
         <v>95</v>
       </c>
-      <c r="J18" t="s">
-        <v>96</v>
-      </c>
       <c r="K18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
         <v>91</v>
       </c>
-      <c r="C19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>92</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" t="s">
         <v>93</v>
       </c>
-      <c r="F19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" t="s">
-        <v>115</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>94</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>95</v>
       </c>
-      <c r="J19" t="s">
-        <v>96</v>
-      </c>
       <c r="K19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" t="s">
-        <v>95</v>
-      </c>
-      <c r="J20" t="s">
-        <v>96</v>
-      </c>
       <c r="K20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" t="s">
+        <v>94</v>
+      </c>
+      <c r="J21" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" t="s">
-        <v>94</v>
-      </c>
-      <c r="I21" t="s">
-        <v>95</v>
-      </c>
-      <c r="J21" t="s">
-        <v>96</v>
-      </c>
       <c r="K21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" t="s">
         <v>91</v>
       </c>
-      <c r="C22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>92</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" t="s">
         <v>93</v>
       </c>
-      <c r="F22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G22" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>94</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>95</v>
       </c>
-      <c r="J22" t="s">
-        <v>96</v>
-      </c>
       <c r="K22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
         <v>91</v>
       </c>
-      <c r="C23" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>92</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" t="s">
         <v>93</v>
       </c>
-      <c r="F23" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" t="s">
-        <v>115</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>94</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>95</v>
       </c>
-      <c r="J23" t="s">
-        <v>96</v>
-      </c>
       <c r="K23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" t="s">
         <v>93</v>
       </c>
-      <c r="F24" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" t="s">
-        <v>115</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>94</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>95</v>
       </c>
-      <c r="J24" t="s">
-        <v>96</v>
-      </c>
       <c r="K24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" t="s">
         <v>93</v>
       </c>
-      <c r="F25" t="s">
-        <v>93</v>
-      </c>
-      <c r="G25" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>94</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>95</v>
       </c>
-      <c r="J25" t="s">
-        <v>96</v>
-      </c>
       <c r="K25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" t="s">
         <v>93</v>
       </c>
-      <c r="F26" t="s">
-        <v>93</v>
-      </c>
-      <c r="G26" t="s">
-        <v>115</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>94</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>95</v>
       </c>
-      <c r="J26" t="s">
-        <v>96</v>
-      </c>
       <c r="K26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" t="s">
         <v>93</v>
       </c>
-      <c r="F27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G27" t="s">
-        <v>115</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>94</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>95</v>
       </c>
-      <c r="J27" t="s">
-        <v>96</v>
-      </c>
       <c r="K27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
         <v>91</v>
       </c>
-      <c r="C28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>92</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" t="s">
+        <v>114</v>
+      </c>
+      <c r="H28" t="s">
         <v>93</v>
       </c>
-      <c r="F28" t="s">
-        <v>93</v>
-      </c>
-      <c r="G28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>94</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>95</v>
       </c>
-      <c r="J28" t="s">
-        <v>96</v>
-      </c>
       <c r="K28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
         <v>91</v>
       </c>
-      <c r="C29" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>92</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29" t="s">
         <v>93</v>
       </c>
-      <c r="F29" t="s">
-        <v>93</v>
-      </c>
-      <c r="G29" t="s">
-        <v>115</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>94</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>95</v>
       </c>
-      <c r="J29" t="s">
-        <v>96</v>
-      </c>
       <c r="K29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" t="s">
         <v>91</v>
       </c>
-      <c r="C30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>92</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" t="s">
         <v>93</v>
       </c>
-      <c r="F30" t="s">
-        <v>93</v>
-      </c>
-      <c r="G30" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>94</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>95</v>
       </c>
-      <c r="J30" t="s">
-        <v>96</v>
-      </c>
       <c r="K30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
         <v>91</v>
       </c>
-      <c r="C31" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>92</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" t="s">
         <v>93</v>
       </c>
-      <c r="F31" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" t="s">
-        <v>115</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>94</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>95</v>
       </c>
-      <c r="J31" t="s">
-        <v>96</v>
-      </c>
       <c r="K31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" t="s">
         <v>91</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" t="s">
+        <v>114</v>
+      </c>
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" t="s">
+        <v>94</v>
+      </c>
+      <c r="J32" t="s">
         <v>95</v>
       </c>
-      <c r="D32" t="s">
-        <v>92</v>
-      </c>
-      <c r="E32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" t="s">
-        <v>93</v>
-      </c>
-      <c r="G32" t="s">
-        <v>115</v>
-      </c>
-      <c r="H32" t="s">
-        <v>94</v>
-      </c>
-      <c r="I32" t="s">
-        <v>95</v>
-      </c>
-      <c r="J32" t="s">
-        <v>96</v>
-      </c>
       <c r="K32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" t="s">
+        <v>94</v>
+      </c>
+      <c r="J33" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" t="s">
-        <v>93</v>
-      </c>
-      <c r="G33" t="s">
-        <v>115</v>
-      </c>
-      <c r="H33" t="s">
-        <v>94</v>
-      </c>
-      <c r="I33" t="s">
-        <v>95</v>
-      </c>
-      <c r="J33" t="s">
-        <v>96</v>
-      </c>
       <c r="K33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>